<commit_message>
Stat server partially in place
Multiple login changes and corrections.
</commit_message>
<xml_diff>
--- a/port_config.xlsx
+++ b/port_config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Account</t>
   </si>
@@ -49,14 +49,25 @@
   </si>
   <si>
     <t>game2</t>
+  </si>
+  <si>
+    <t>Stat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,30 +493,42 @@
         <v>7702</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>21000</v>
-      </c>
-      <c r="C11">
-        <v>21002</v>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7800</v>
+      </c>
+      <c r="C10">
+        <v>7802</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>21100</v>
+        <v>21000</v>
       </c>
       <c r="C12">
         <v>21002</v>
       </c>
     </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>21100</v>
+      </c>
+      <c r="C13">
+        <v>21002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Moved serialize and added notification
Reorganization of file structure
Server stack updated to include the notification server.
Notification server talks to Game and Login
Packets in place.
</commit_message>
<xml_diff>
--- a/port_config.xlsx
+++ b/port_config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Account</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Stat</t>
+  </si>
+  <si>
+    <t>Notification</t>
   </si>
 </sst>
 </file>
@@ -392,13 +395,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
@@ -506,23 +512,34 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7900</v>
+      </c>
+      <c r="C12">
+        <v>7902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B15">
         <v>21000</v>
       </c>
-      <c r="C12">
+      <c r="C15">
         <v>21002</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B16">
         <v>21100</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>21002</v>
       </c>
     </row>

</xml_diff>